<commit_message>
rebuild all for sidebars
</commit_message>
<xml_diff>
--- a/source/class_schedule.xlsx
+++ b/source/class_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/unifyingdatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7841BD91-8140-9C4D-9119-EAB11D931E8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D200B9-4491-EC4E-BF97-F7F8E74659F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3360" yWindow="580" windowWidth="35040" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -171,19 +171,6 @@
     <t>Wed, Apr 15</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Angrist and Piscke </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="SFBX1200"/>
-      </rPr>
-      <t xml:space="preserve">Pages 222-247. </t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">`Matching Methods for Causal Inference: A Review and a Look Forward &lt;https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2943670/&gt;`_ </t>
   </si>
   <si>
@@ -344,6 +331,19 @@
     <t>- `Interpreting Indicator Vars &lt;interpreting_indicator_vars.ipynb&gt;`_
 - `Fixed Effects v. Hierarchical Models &lt;fixed_effects_v_hierarchical.ipynb&gt;`_
 - `Fixed Effects &lt;fixed_effects.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <r>
+      <t>Angrist and Piscke (MM), Chapter 5 (pp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="SFBX1200"/>
+      </rPr>
+      <t xml:space="preserve"> 178-208) </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -750,7 +750,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -785,7 +785,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" ht="85">
+    <row r="3" spans="1:4" ht="71">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -793,13 +793,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="153">
+    </row>
+    <row r="4" spans="1:4" ht="85">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -807,10 +807,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -822,7 +822,7 @@
       </c>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:4" ht="85">
+    <row r="6" spans="1:4" ht="57">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -830,13 +830,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="136">
+    </row>
+    <row r="7" spans="1:4" ht="85">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -844,13 +844,13 @@
         <v>11</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="119">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="85">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -858,13 +858,13 @@
         <v>11</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="153">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="85">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -872,38 +872,38 @@
         <v>12</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="68">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="51">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="85">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="51">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -919,10 +919,10 @@
         <v>14</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="85">
@@ -930,13 +930,13 @@
         <v>29</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="85">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="68">
       <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
@@ -944,10 +944,10 @@
         <v>13</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="34">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17">
       <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
@@ -955,7 +955,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17">
@@ -968,7 +968,7 @@
       <c r="C17" s="11"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="204">
+    <row r="18" spans="1:4" ht="119">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
@@ -976,7 +976,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1001,32 +1001,32 @@
         <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="153">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="119">
       <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="409.6">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="306">
       <c r="A23" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1046,10 +1046,10 @@
         <v>41</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1057,10 +1057,10 @@
         <v>42</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1068,10 +1068,10 @@
         <v>43</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:4">

</xml_diff>